<commit_message>
Changed 'Storage' to 'Battery'.
</commit_message>
<xml_diff>
--- a/Calc/CO2_Calc.xlsx
+++ b/Calc/CO2_Calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFDD542-4825-49C5-ACC4-D277626AA786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F46E99-CD40-4582-A11E-B61A0EE8CC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{738DFCFF-3A0D-4B61-9084-C2C50E31EE06}"/>
   </bookViews>
@@ -16,11 +16,11 @@
     <sheet name="CO2" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="CO2_gen_Battery">'CO2'!$G$5</definedName>
     <definedName name="CO2_gen_Coal">'CO2'!$F$5</definedName>
     <definedName name="CO2_gen_Gas">'CO2'!$E$5</definedName>
     <definedName name="CO2_gen_Nuclear">'CO2'!$D$5</definedName>
     <definedName name="CO2_gen_Solar">'CO2'!$B$5</definedName>
-    <definedName name="CO2_gen_Storage">'CO2'!$G$5</definedName>
     <definedName name="CO2_gen_Wind">'CO2'!$C$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -58,9 +58,6 @@
     <t>Solar</t>
   </si>
   <si>
-    <t>Storage</t>
-  </si>
-  <si>
     <t>Wind</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>CO2_gen</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -411,9 +411,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -451,7 +451,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -557,7 +557,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -699,7 +699,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -711,7 +711,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
@@ -723,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.85">
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.85">
@@ -731,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -743,12 +743,12 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="str">
         <f>$A4 &amp; "_" &amp; B$2</f>
@@ -792,12 +792,12 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>CO2_gen_Storage</v>
+        <v>CO2_gen_Battery</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <f>B3/1000000000</f>
@@ -826,12 +826,12 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -845,10 +845,10 @@
         <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.85">
@@ -857,10 +857,10 @@
         <v>0.11125</v>
       </c>
       <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
         <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.85">
@@ -869,7 +869,7 @@
         <v>0.11125</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>